<commit_message>
Adding manually curated fixes
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2011 Data/BogUpper5-R10.xlsx
+++ b/Data/phenotypic data/RawData/2011 Data/BogUpper5-R10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="5140" windowWidth="11120" windowHeight="8900"/>
+    <workbookView xWindow="3600" yWindow="0" windowWidth="11120" windowHeight="8900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3525" uniqueCount="142">
   <si>
     <t>Berry</t>
   </si>
@@ -636,9 +636,6 @@
     <t>Row/Col: R10 C40</t>
   </si>
   <si>
-    <t>pinted</t>
-  </si>
-  <si>
     <t xml:space="preserve">small </t>
   </si>
   <si>
@@ -1015,6 +1012,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1024,6 +1024,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1032,10 +1033,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1371,31 +1368,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A512" workbookViewId="0">
-      <selection activeCell="E523" sqref="E523"/>
+    <sheetView tabSelected="1" topLeftCell="A566" workbookViewId="0">
+      <selection activeCell="G599" sqref="G599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="7.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="6.5" style="4" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="7.5" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5" style="5" customWidth="1"/>
-    <col min="17" max="19" width="8.5" style="3" customWidth="1"/>
-    <col min="20" max="20" width="9.5" style="4" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="4" customWidth="1"/>
-    <col min="22" max="16384" width="10" style="3"/>
+    <col min="2" max="2" width="5.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="3" customWidth="1"/>
+    <col min="5" max="6" width="3.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="3" customWidth="1"/>
+    <col min="8" max="9" width="6.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="4.5" style="4" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="50" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="8" style="5" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="8.5" style="3" customWidth="1"/>
+    <col min="19" max="19" width="7" style="3" customWidth="1"/>
+    <col min="20" max="20" width="8" style="4" customWidth="1"/>
+    <col min="21" max="21" width="6.83203125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="5.1640625" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="10" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.5" customHeight="1">
@@ -1445,53 +1444,53 @@
       <c r="U2" s="17"/>
     </row>
     <row r="3" spans="1:21" ht="32.25" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
       <c r="U3" s="37"/>
     </row>
     <row r="4" spans="1:21" ht="30.75" customHeight="1">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
       <c r="U4" s="37"/>
     </row>
     <row r="5" spans="1:21" ht="19.5" customHeight="1">
@@ -1603,28 +1602,28 @@
       <c r="U9" s="17"/>
     </row>
     <row r="10" spans="1:21" ht="30.75" customHeight="1">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="59"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
       <c r="U10" s="32"/>
     </row>
     <row r="11" spans="1:21" ht="16.5" customHeight="1">
@@ -1797,78 +1796,78 @@
       <c r="B19" s="9"/>
     </row>
     <row r="20" spans="1:22" ht="18.75" customHeight="1">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="58"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="59"/>
+      <c r="Q20" s="59"/>
+      <c r="R20" s="59"/>
+      <c r="S20" s="59"/>
+      <c r="T20" s="59"/>
       <c r="U20" s="32"/>
     </row>
     <row r="21" spans="1:22" ht="27.75" customHeight="1">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="58"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="58"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="59"/>
       <c r="U21" s="32"/>
     </row>
     <row r="22" spans="1:22" ht="33" customHeight="1">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
-      <c r="P22" s="58"/>
-      <c r="Q22" s="58"/>
-      <c r="R22" s="58"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="58"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="59"/>
+      <c r="T22" s="59"/>
       <c r="U22" s="32"/>
     </row>
     <row r="24" spans="1:22" ht="19.5" customHeight="1">
@@ -1941,10 +1940,10 @@
       <c r="L32" s="21"/>
       <c r="M32" s="17"/>
       <c r="N32" s="48"/>
-      <c r="O32" s="55" t="s">
+      <c r="O32" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P32" s="55"/>
+      <c r="P32" s="56"/>
       <c r="Q32" s="5"/>
       <c r="T32" s="3"/>
       <c r="V32" s="17"/>
@@ -1959,11 +1958,11 @@
         <v>16</v>
       </c>
       <c r="J33" s="24"/>
-      <c r="K33" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
+      <c r="K33" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" s="57"/>
+      <c r="M33" s="57"/>
       <c r="N33" s="52" t="s">
         <v>23</v>
       </c>
@@ -2117,11 +2116,11 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
       <c r="D36" s="40"/>
       <c r="E36" s="40"/>
       <c r="F36" s="40"/>
@@ -2295,7 +2294,7 @@
         <v>3</v>
       </c>
       <c r="H39" s="26">
-        <v>9.6999999999999993</v>
+        <v>11</v>
       </c>
       <c r="I39" s="26"/>
       <c r="J39" s="15">
@@ -2426,10 +2425,10 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="H41" s="3">
-        <v>4.3</v>
+        <v>1</v>
       </c>
       <c r="I41" s="3">
-        <v>4.0999999999999996</v>
+        <v>5.5</v>
       </c>
       <c r="J41" s="4">
         <v>0.122</v>
@@ -2810,11 +2809,11 @@
       <c r="A47" s="4"/>
     </row>
     <row r="48" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A48" s="60" t="s">
+      <c r="A48" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="60"/>
-      <c r="C48" s="60"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
@@ -3482,6 +3481,12 @@
       <c r="T58" s="15" t="s">
         <v>72</v>
       </c>
+      <c r="U58" s="4">
+        <v>17</v>
+      </c>
+      <c r="V58" s="38" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="60" spans="1:22" ht="19.5" customHeight="1">
       <c r="A60" s="35" t="s">
@@ -3499,10 +3504,10 @@
       <c r="L60" s="21"/>
       <c r="M60" s="17"/>
       <c r="N60" s="48"/>
-      <c r="O60" s="55" t="s">
+      <c r="O60" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P60" s="55"/>
+      <c r="P60" s="56"/>
       <c r="Q60" s="5"/>
       <c r="T60" s="3"/>
       <c r="V60" s="17"/>
@@ -3517,11 +3522,11 @@
         <v>16</v>
       </c>
       <c r="J61" s="24"/>
-      <c r="K61" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L61" s="56"/>
-      <c r="M61" s="56"/>
+      <c r="K61" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L61" s="57"/>
+      <c r="M61" s="57"/>
       <c r="N61" s="52" t="s">
         <v>23</v>
       </c>
@@ -3675,11 +3680,11 @@
       </c>
     </row>
     <row r="64" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A64" s="57" t="s">
+      <c r="A64" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="57"/>
-      <c r="C64" s="57"/>
+      <c r="B64" s="55"/>
+      <c r="C64" s="55"/>
       <c r="D64" s="40"/>
       <c r="E64" s="40"/>
       <c r="F64" s="40"/>
@@ -3834,10 +3839,10 @@
         <v>5</v>
       </c>
       <c r="C67" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E67" s="3">
         <v>1</v>
@@ -4127,7 +4132,7 @@
         <v>2.23</v>
       </c>
       <c r="N71" s="50">
-        <v>2.7</v>
+        <v>2.74</v>
       </c>
       <c r="O71" s="33" t="s">
         <v>6</v>
@@ -4356,11 +4361,11 @@
       </c>
     </row>
     <row r="76" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A76" s="57" t="s">
+      <c r="A76" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="B76" s="57"/>
-      <c r="C76" s="57"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="55"/>
     </row>
     <row r="77" spans="1:22" ht="19.5" customHeight="1">
       <c r="A77" s="3">
@@ -5043,10 +5048,10 @@
       <c r="L88" s="21"/>
       <c r="M88" s="17"/>
       <c r="N88" s="48"/>
-      <c r="O88" s="55" t="s">
+      <c r="O88" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P88" s="55"/>
+      <c r="P88" s="56"/>
       <c r="Q88" s="5"/>
       <c r="T88" s="3"/>
       <c r="V88" s="17"/>
@@ -5061,11 +5066,11 @@
         <v>16</v>
       </c>
       <c r="J89" s="24"/>
-      <c r="K89" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L89" s="56"/>
-      <c r="M89" s="56"/>
+      <c r="K89" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L89" s="57"/>
+      <c r="M89" s="57"/>
       <c r="N89" s="52" t="s">
         <v>23</v>
       </c>
@@ -5219,11 +5224,11 @@
       </c>
     </row>
     <row r="92" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A92" s="57" t="s">
+      <c r="A92" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B92" s="57"/>
-      <c r="C92" s="57"/>
+      <c r="B92" s="55"/>
+      <c r="C92" s="55"/>
       <c r="D92" s="40"/>
       <c r="E92" s="40"/>
       <c r="F92" s="40"/>
@@ -5390,7 +5395,7 @@
         <v>0</v>
       </c>
       <c r="G95" s="3">
-        <v>2.5499999999999998</v>
+        <v>2.35</v>
       </c>
       <c r="H95" s="3">
         <v>3</v>
@@ -5647,7 +5652,7 @@
         <v>1</v>
       </c>
       <c r="E99" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" s="3">
         <v>1</v>
@@ -5894,11 +5899,11 @@
       </c>
     </row>
     <row r="104" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A104" s="57" t="s">
+      <c r="A104" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B104" s="57"/>
-      <c r="C104" s="57"/>
+      <c r="B104" s="55"/>
+      <c r="C104" s="55"/>
     </row>
     <row r="105" spans="1:22" ht="19.5" customHeight="1">
       <c r="A105" s="3">
@@ -5926,7 +5931,7 @@
         <v>1.5</v>
       </c>
       <c r="J105" s="45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K105" s="4">
         <v>20.96</v>
@@ -5953,7 +5958,7 @@
         <v>71</v>
       </c>
       <c r="S105" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T105" s="15" t="s">
         <v>75</v>
@@ -6018,7 +6023,7 @@
         <v>71</v>
       </c>
       <c r="S106" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T106" s="15" t="s">
         <v>71</v>
@@ -6548,6 +6553,41 @@
       </c>
       <c r="V114" s="26" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="115" spans="1:22" ht="19.5" customHeight="1">
+      <c r="A115" s="3">
+        <v>11</v>
+      </c>
+      <c r="B115" s="3">
+        <v>5</v>
+      </c>
+      <c r="C115" s="3">
+        <v>3</v>
+      </c>
+      <c r="D115" s="3">
+        <v>2</v>
+      </c>
+      <c r="E115" s="3">
+        <v>1</v>
+      </c>
+      <c r="F115" s="3">
+        <v>1</v>
+      </c>
+      <c r="G115" s="3">
+        <v>4.53</v>
+      </c>
+      <c r="H115" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="K115" s="4">
+        <v>25.14</v>
+      </c>
+      <c r="L115" s="4">
+        <v>18.61</v>
+      </c>
+      <c r="M115" s="4">
+        <v>2.81</v>
       </c>
     </row>
     <row r="116" spans="1:22" ht="19.5" customHeight="1">
@@ -6566,10 +6606,10 @@
       <c r="L116" s="21"/>
       <c r="M116" s="17"/>
       <c r="N116" s="48"/>
-      <c r="O116" s="55" t="s">
+      <c r="O116" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P116" s="55"/>
+      <c r="P116" s="56"/>
       <c r="Q116" s="5"/>
       <c r="T116" s="3"/>
       <c r="V116" s="17"/>
@@ -6584,11 +6624,11 @@
         <v>16</v>
       </c>
       <c r="J117" s="24"/>
-      <c r="K117" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L117" s="56"/>
-      <c r="M117" s="56"/>
+      <c r="K117" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L117" s="57"/>
+      <c r="M117" s="57"/>
       <c r="N117" s="52" t="s">
         <v>23</v>
       </c>
@@ -6742,11 +6782,11 @@
       </c>
     </row>
     <row r="120" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A120" s="57" t="s">
+      <c r="A120" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="B120" s="57"/>
-      <c r="C120" s="57"/>
+      <c r="B120" s="55"/>
+      <c r="C120" s="55"/>
       <c r="D120" s="40"/>
       <c r="E120" s="40"/>
       <c r="F120" s="40"/>
@@ -6981,7 +7021,7 @@
         <v>1</v>
       </c>
       <c r="G124" s="3">
-        <v>4.8899999999999997</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H124" s="3">
         <v>2.5</v>
@@ -7423,11 +7463,11 @@
       </c>
     </row>
     <row r="132" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A132" s="57" t="s">
+      <c r="A132" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="B132" s="57"/>
-      <c r="C132" s="57"/>
+      <c r="B132" s="55"/>
+      <c r="C132" s="55"/>
     </row>
     <row r="133" spans="1:22" ht="19.5" customHeight="1">
       <c r="A133" s="3">
@@ -7520,7 +7560,7 @@
         <v>4</v>
       </c>
       <c r="J134" s="45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K134" s="4">
         <v>19.8</v>
@@ -8098,10 +8138,10 @@
       <c r="L144" s="21"/>
       <c r="M144" s="17"/>
       <c r="N144" s="48"/>
-      <c r="O144" s="55" t="s">
+      <c r="O144" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P144" s="55"/>
+      <c r="P144" s="56"/>
       <c r="Q144" s="5"/>
       <c r="T144" s="3"/>
       <c r="V144" s="17"/>
@@ -8116,11 +8156,11 @@
         <v>16</v>
       </c>
       <c r="J145" s="24"/>
-      <c r="K145" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L145" s="56"/>
-      <c r="M145" s="56"/>
+      <c r="K145" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L145" s="57"/>
+      <c r="M145" s="57"/>
       <c r="N145" s="52" t="s">
         <v>23</v>
       </c>
@@ -8274,11 +8314,11 @@
       </c>
     </row>
     <row r="148" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A148" s="57" t="s">
+      <c r="A148" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="B148" s="57"/>
-      <c r="C148" s="57"/>
+      <c r="B148" s="55"/>
+      <c r="C148" s="55"/>
       <c r="D148" s="40"/>
       <c r="E148" s="40"/>
       <c r="F148" s="40"/>
@@ -8452,7 +8492,7 @@
         <v>6.69</v>
       </c>
       <c r="H151" s="3">
-        <v>3.6</v>
+        <v>3.9</v>
       </c>
       <c r="J151" s="4">
         <v>8.4000000000000005E-2</v>
@@ -8757,7 +8797,7 @@
         <v>25</v>
       </c>
       <c r="V155" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="156" spans="1:23" ht="19.5" customHeight="1">
@@ -8956,11 +8996,11 @@
       </c>
     </row>
     <row r="160" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A160" s="57" t="s">
+      <c r="A160" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="B160" s="57"/>
-      <c r="C160" s="57"/>
+      <c r="B160" s="55"/>
+      <c r="C160" s="55"/>
     </row>
     <row r="161" spans="1:22" ht="19.5" customHeight="1">
       <c r="A161" s="3">
@@ -9511,7 +9551,7 @@
         <v>0.7</v>
       </c>
       <c r="J169" s="45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K169" s="4">
         <v>21.2</v>
@@ -9561,7 +9601,7 @@
         <v>0</v>
       </c>
       <c r="D170" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E170" s="3">
         <v>0</v>
@@ -9629,10 +9669,10 @@
       <c r="L172" s="21"/>
       <c r="M172" s="17"/>
       <c r="N172" s="48"/>
-      <c r="O172" s="55" t="s">
+      <c r="O172" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P172" s="55"/>
+      <c r="P172" s="56"/>
       <c r="Q172" s="5"/>
       <c r="T172" s="3"/>
       <c r="V172" s="17"/>
@@ -9647,11 +9687,11 @@
         <v>16</v>
       </c>
       <c r="J173" s="24"/>
-      <c r="K173" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L173" s="56"/>
-      <c r="M173" s="56"/>
+      <c r="K173" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L173" s="57"/>
+      <c r="M173" s="57"/>
       <c r="N173" s="52" t="s">
         <v>23</v>
       </c>
@@ -9805,11 +9845,11 @@
       </c>
     </row>
     <row r="176" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A176" s="57" t="s">
+      <c r="A176" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="B176" s="57"/>
-      <c r="C176" s="57"/>
+      <c r="B176" s="55"/>
+      <c r="C176" s="55"/>
       <c r="D176" s="40"/>
       <c r="E176" s="40"/>
       <c r="F176" s="40"/>
@@ -10233,10 +10273,10 @@
         <v>2</v>
       </c>
       <c r="E183" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F183" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G183" s="3">
         <v>5.4</v>
@@ -10486,11 +10526,11 @@
       </c>
     </row>
     <row r="188" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A188" s="57" t="s">
+      <c r="A188" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="B188" s="57"/>
-      <c r="C188" s="57"/>
+      <c r="B188" s="55"/>
+      <c r="C188" s="55"/>
     </row>
     <row r="189" spans="1:22" ht="19.5" customHeight="1">
       <c r="A189" s="3">
@@ -11161,10 +11201,10 @@
       <c r="L200" s="21"/>
       <c r="M200" s="17"/>
       <c r="N200" s="48"/>
-      <c r="O200" s="55" t="s">
+      <c r="O200" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P200" s="55"/>
+      <c r="P200" s="56"/>
       <c r="Q200" s="5"/>
       <c r="T200" s="3"/>
       <c r="V200" s="17"/>
@@ -11179,11 +11219,11 @@
         <v>16</v>
       </c>
       <c r="J201" s="24"/>
-      <c r="K201" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L201" s="56"/>
-      <c r="M201" s="56"/>
+      <c r="K201" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L201" s="57"/>
+      <c r="M201" s="57"/>
       <c r="N201" s="52" t="s">
         <v>23</v>
       </c>
@@ -11337,11 +11377,11 @@
       </c>
     </row>
     <row r="204" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A204" s="57" t="s">
+      <c r="A204" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="B204" s="57"/>
-      <c r="C204" s="57"/>
+      <c r="B204" s="55"/>
+      <c r="C204" s="55"/>
       <c r="D204" s="40"/>
       <c r="E204" s="40"/>
       <c r="F204" s="40"/>
@@ -12030,11 +12070,11 @@
       </c>
     </row>
     <row r="216" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A216" s="57" t="s">
+      <c r="A216" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="B216" s="57"/>
-      <c r="C216" s="57"/>
+      <c r="B216" s="55"/>
+      <c r="C216" s="55"/>
     </row>
     <row r="217" spans="1:22" ht="19.5" customHeight="1">
       <c r="A217" s="3">
@@ -12443,10 +12483,10 @@
         <v>2</v>
       </c>
       <c r="E223" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F223" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G223" s="3">
         <v>5.39</v>
@@ -12705,10 +12745,10 @@
       <c r="L228" s="21"/>
       <c r="M228" s="17"/>
       <c r="N228" s="48"/>
-      <c r="O228" s="55" t="s">
+      <c r="O228" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P228" s="55"/>
+      <c r="P228" s="56"/>
       <c r="Q228" s="5"/>
       <c r="T228" s="3"/>
       <c r="V228" s="17"/>
@@ -12723,11 +12763,11 @@
         <v>16</v>
       </c>
       <c r="J229" s="24"/>
-      <c r="K229" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L229" s="56"/>
-      <c r="M229" s="56"/>
+      <c r="K229" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L229" s="57"/>
+      <c r="M229" s="57"/>
       <c r="N229" s="52" t="s">
         <v>23</v>
       </c>
@@ -12881,11 +12921,11 @@
       </c>
     </row>
     <row r="232" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A232" s="57" t="s">
+      <c r="A232" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="B232" s="57"/>
-      <c r="C232" s="57"/>
+      <c r="B232" s="55"/>
+      <c r="C232" s="55"/>
       <c r="D232" s="40"/>
       <c r="E232" s="40"/>
       <c r="F232" s="40"/>
@@ -13553,11 +13593,11 @@
       </c>
     </row>
     <row r="244" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A244" s="57" t="s">
+      <c r="A244" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="B244" s="57"/>
-      <c r="C244" s="57"/>
+      <c r="B244" s="55"/>
+      <c r="C244" s="55"/>
     </row>
     <row r="245" spans="1:22" ht="19.5" customHeight="1">
       <c r="A245" s="3">
@@ -13665,7 +13705,7 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="N246" s="50">
-        <v>2.5299999999999998</v>
+        <v>2.52</v>
       </c>
       <c r="O246" s="43" t="s">
         <v>14</v>
@@ -13721,10 +13761,10 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="K247" s="4">
-        <v>22.91</v>
+        <v>23.23</v>
       </c>
       <c r="L247" s="4">
-        <v>19.25</v>
+        <v>19.52</v>
       </c>
       <c r="M247" s="4">
         <v>2.85</v>
@@ -14129,7 +14169,7 @@
         <v>2.12</v>
       </c>
       <c r="N253" s="50">
-        <v>2.79</v>
+        <v>2.7</v>
       </c>
       <c r="O253" s="43" t="s">
         <v>6</v>
@@ -14237,10 +14277,10 @@
       <c r="L256" s="21"/>
       <c r="M256" s="17"/>
       <c r="N256" s="48"/>
-      <c r="O256" s="55" t="s">
+      <c r="O256" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P256" s="55"/>
+      <c r="P256" s="56"/>
       <c r="Q256" s="5"/>
       <c r="T256" s="3"/>
       <c r="V256" s="17"/>
@@ -14255,11 +14295,11 @@
         <v>16</v>
       </c>
       <c r="J257" s="24"/>
-      <c r="K257" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L257" s="56"/>
-      <c r="M257" s="56"/>
+      <c r="K257" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L257" s="57"/>
+      <c r="M257" s="57"/>
       <c r="N257" s="52" t="s">
         <v>23</v>
       </c>
@@ -14413,11 +14453,11 @@
       </c>
     </row>
     <row r="260" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A260" s="57" t="s">
+      <c r="A260" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B260" s="57"/>
-      <c r="C260" s="57"/>
+      <c r="B260" s="55"/>
+      <c r="C260" s="55"/>
       <c r="D260" s="40"/>
       <c r="E260" s="40"/>
       <c r="F260" s="40"/>
@@ -14667,7 +14707,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="N264" s="50">
-        <v>2.4</v>
+        <v>2.37</v>
       </c>
       <c r="O264" s="43" t="s">
         <v>6</v>
@@ -14989,7 +15029,7 @@
         <v>18.25</v>
       </c>
       <c r="M269" s="4">
-        <v>2.72</v>
+        <v>2.73</v>
       </c>
       <c r="N269" s="50">
         <v>2.37</v>
@@ -15085,11 +15125,11 @@
       </c>
     </row>
     <row r="272" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A272" s="57" t="s">
+      <c r="A272" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="B272" s="57"/>
-      <c r="C272" s="57"/>
+      <c r="B272" s="55"/>
+      <c r="C272" s="55"/>
     </row>
     <row r="273" spans="1:22" ht="19.5" customHeight="1">
       <c r="A273" s="3">
@@ -15345,7 +15385,7 @@
         <v>2</v>
       </c>
       <c r="T276" s="44" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="U276" s="4">
         <v>19</v>
@@ -15466,7 +15506,7 @@
         <v>14</v>
       </c>
       <c r="Q278" s="38" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="R278" s="38" t="s">
         <v>71</v>
@@ -15478,7 +15518,7 @@
         <v>71</v>
       </c>
       <c r="U278" s="4">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="V278" s="38" t="s">
         <v>73</v>
@@ -15754,10 +15794,10 @@
       <c r="L284" s="21"/>
       <c r="M284" s="17"/>
       <c r="N284" s="48"/>
-      <c r="O284" s="55" t="s">
+      <c r="O284" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P284" s="55"/>
+      <c r="P284" s="56"/>
       <c r="Q284" s="5"/>
       <c r="T284" s="3"/>
       <c r="V284" s="17"/>
@@ -15772,11 +15812,11 @@
         <v>16</v>
       </c>
       <c r="J285" s="24"/>
-      <c r="K285" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L285" s="56"/>
-      <c r="M285" s="56"/>
+      <c r="K285" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L285" s="57"/>
+      <c r="M285" s="57"/>
       <c r="N285" s="52" t="s">
         <v>23</v>
       </c>
@@ -15930,11 +15970,11 @@
       </c>
     </row>
     <row r="288" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A288" s="57" t="s">
+      <c r="A288" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="B288" s="57"/>
-      <c r="C288" s="57"/>
+      <c r="B288" s="55"/>
+      <c r="C288" s="55"/>
       <c r="D288" s="40"/>
       <c r="E288" s="40"/>
       <c r="F288" s="40"/>
@@ -16255,16 +16295,16 @@
         <v>61</v>
       </c>
       <c r="P293" s="43" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="Q293" s="38" t="s">
         <v>80</v>
       </c>
       <c r="R293" s="38" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="S293" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T293" s="44" t="s">
         <v>71</v>
@@ -16605,11 +16645,11 @@
       </c>
     </row>
     <row r="300" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A300" s="57" t="s">
+      <c r="A300" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="B300" s="57"/>
-      <c r="C300" s="57"/>
+      <c r="B300" s="55"/>
+      <c r="C300" s="55"/>
     </row>
     <row r="301" spans="1:22" ht="19.5" customHeight="1">
       <c r="A301" s="3">
@@ -17169,7 +17209,7 @@
         <v>16.59</v>
       </c>
       <c r="M309" s="4">
-        <v>8.44</v>
+        <v>2.44</v>
       </c>
       <c r="N309" s="50">
         <v>2.7</v>
@@ -17231,7 +17271,7 @@
         <v>22.8</v>
       </c>
       <c r="L310" s="4">
-        <v>19.7</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="M310" s="4">
         <v>1.84</v>
@@ -17280,10 +17320,10 @@
       <c r="L312" s="21"/>
       <c r="M312" s="17"/>
       <c r="N312" s="48"/>
-      <c r="O312" s="55" t="s">
+      <c r="O312" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P312" s="55"/>
+      <c r="P312" s="56"/>
       <c r="Q312" s="5"/>
       <c r="T312" s="3"/>
       <c r="V312" s="17"/>
@@ -17298,11 +17338,11 @@
         <v>16</v>
       </c>
       <c r="J313" s="24"/>
-      <c r="K313" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L313" s="56"/>
-      <c r="M313" s="56"/>
+      <c r="K313" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L313" s="57"/>
+      <c r="M313" s="57"/>
       <c r="N313" s="52" t="s">
         <v>23</v>
       </c>
@@ -17456,11 +17496,11 @@
       </c>
     </row>
     <row r="316" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A316" s="57" t="s">
+      <c r="A316" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="B316" s="57"/>
-      <c r="C316" s="57"/>
+      <c r="B316" s="55"/>
+      <c r="C316" s="55"/>
       <c r="D316" s="40"/>
       <c r="E316" s="40"/>
       <c r="F316" s="40"/>
@@ -18134,11 +18174,11 @@
       </c>
     </row>
     <row r="328" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A328" s="57" t="s">
+      <c r="A328" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="B328" s="57"/>
-      <c r="C328" s="57"/>
+      <c r="B328" s="55"/>
+      <c r="C328" s="55"/>
     </row>
     <row r="329" spans="1:22" ht="19.5" customHeight="1">
       <c r="A329" s="3">
@@ -18809,10 +18849,10 @@
       <c r="L340" s="21"/>
       <c r="M340" s="17"/>
       <c r="N340" s="48"/>
-      <c r="O340" s="55" t="s">
+      <c r="O340" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P340" s="55"/>
+      <c r="P340" s="56"/>
       <c r="Q340" s="5"/>
       <c r="T340" s="3"/>
       <c r="V340" s="17"/>
@@ -18827,11 +18867,11 @@
         <v>16</v>
       </c>
       <c r="J341" s="24"/>
-      <c r="K341" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L341" s="56"/>
-      <c r="M341" s="56"/>
+      <c r="K341" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L341" s="57"/>
+      <c r="M341" s="57"/>
       <c r="N341" s="52" t="s">
         <v>23</v>
       </c>
@@ -18985,11 +19025,11 @@
       </c>
     </row>
     <row r="344" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A344" s="57" t="s">
+      <c r="A344" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="B344" s="57"/>
-      <c r="C344" s="57"/>
+      <c r="B344" s="55"/>
+      <c r="C344" s="55"/>
       <c r="D344" s="40"/>
       <c r="E344" s="40"/>
       <c r="F344" s="40"/>
@@ -19660,11 +19700,11 @@
       </c>
     </row>
     <row r="356" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A356" s="57" t="s">
+      <c r="A356" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="B356" s="57"/>
-      <c r="C356" s="57"/>
+      <c r="B356" s="55"/>
+      <c r="C356" s="55"/>
     </row>
     <row r="357" spans="1:22" ht="19.5" customHeight="1">
       <c r="A357" s="3">
@@ -20038,7 +20078,7 @@
         <v>14</v>
       </c>
       <c r="Q362" s="38" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="R362" s="38" t="s">
         <v>71</v>
@@ -20332,10 +20372,10 @@
       <c r="L368" s="21"/>
       <c r="M368" s="17"/>
       <c r="N368" s="48"/>
-      <c r="O368" s="55" t="s">
+      <c r="O368" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P368" s="55"/>
+      <c r="P368" s="56"/>
       <c r="Q368" s="5"/>
       <c r="T368" s="3"/>
       <c r="V368" s="17"/>
@@ -20350,11 +20390,11 @@
         <v>16</v>
       </c>
       <c r="J369" s="24"/>
-      <c r="K369" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L369" s="56"/>
-      <c r="M369" s="56"/>
+      <c r="K369" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L369" s="57"/>
+      <c r="M369" s="57"/>
       <c r="N369" s="52" t="s">
         <v>23</v>
       </c>
@@ -20508,11 +20548,11 @@
       </c>
     </row>
     <row r="372" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A372" s="57" t="s">
+      <c r="A372" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="B372" s="57"/>
-      <c r="C372" s="57"/>
+      <c r="B372" s="55"/>
+      <c r="C372" s="55"/>
       <c r="D372" s="40"/>
       <c r="E372" s="40"/>
       <c r="F372" s="40"/>
@@ -21177,11 +21217,11 @@
       </c>
     </row>
     <row r="384" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A384" s="57" t="s">
+      <c r="A384" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="B384" s="57"/>
-      <c r="C384" s="57"/>
+      <c r="B384" s="55"/>
+      <c r="C384" s="55"/>
     </row>
     <row r="385" spans="1:22" ht="19.5" customHeight="1">
       <c r="A385" s="3">
@@ -21858,10 +21898,10 @@
       <c r="L397" s="21"/>
       <c r="M397" s="17"/>
       <c r="N397" s="48"/>
-      <c r="O397" s="55" t="s">
+      <c r="O397" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P397" s="55"/>
+      <c r="P397" s="56"/>
       <c r="Q397" s="5"/>
       <c r="T397" s="3"/>
       <c r="V397" s="17"/>
@@ -21876,11 +21916,11 @@
         <v>16</v>
       </c>
       <c r="J398" s="24"/>
-      <c r="K398" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L398" s="56"/>
-      <c r="M398" s="56"/>
+      <c r="K398" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L398" s="57"/>
+      <c r="M398" s="57"/>
       <c r="N398" s="52" t="s">
         <v>23</v>
       </c>
@@ -22034,11 +22074,11 @@
       </c>
     </row>
     <row r="401" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A401" s="57" t="s">
+      <c r="A401" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="B401" s="57"/>
-      <c r="C401" s="57"/>
+      <c r="B401" s="55"/>
+      <c r="C401" s="55"/>
       <c r="D401" s="40"/>
       <c r="E401" s="40"/>
       <c r="F401" s="40"/>
@@ -22238,7 +22278,7 @@
         <v>71</v>
       </c>
       <c r="R404" s="38" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="S404" s="3">
         <v>2</v>
@@ -22368,7 +22408,7 @@
         <v>80</v>
       </c>
       <c r="R406" s="38" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="S406" s="3">
         <v>2</v>
@@ -22427,7 +22467,7 @@
         <v>61</v>
       </c>
       <c r="P407" s="43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q407" s="38" t="s">
         <v>80</v>
@@ -22709,11 +22749,11 @@
       </c>
     </row>
     <row r="413" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A413" s="57" t="s">
+      <c r="A413" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="B413" s="57"/>
-      <c r="C413" s="57"/>
+      <c r="B413" s="55"/>
+      <c r="C413" s="55"/>
     </row>
     <row r="414" spans="1:22" ht="19.5" customHeight="1">
       <c r="A414" s="3">
@@ -23387,10 +23427,10 @@
       <c r="L426" s="21"/>
       <c r="M426" s="17"/>
       <c r="N426" s="48"/>
-      <c r="O426" s="55" t="s">
+      <c r="O426" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P426" s="55"/>
+      <c r="P426" s="56"/>
       <c r="Q426" s="5"/>
       <c r="T426" s="3"/>
       <c r="V426" s="17"/>
@@ -23405,11 +23445,11 @@
         <v>16</v>
       </c>
       <c r="J427" s="24"/>
-      <c r="K427" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L427" s="56"/>
-      <c r="M427" s="56"/>
+      <c r="K427" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L427" s="57"/>
+      <c r="M427" s="57"/>
       <c r="N427" s="52" t="s">
         <v>23</v>
       </c>
@@ -23563,11 +23603,11 @@
       </c>
     </row>
     <row r="430" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A430" s="57" t="s">
+      <c r="A430" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="B430" s="57"/>
-      <c r="C430" s="57"/>
+      <c r="B430" s="55"/>
+      <c r="C430" s="55"/>
       <c r="D430" s="40"/>
       <c r="E430" s="40"/>
       <c r="F430" s="40"/>
@@ -24256,11 +24296,11 @@
       </c>
     </row>
     <row r="442" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A442" s="57" t="s">
+      <c r="A442" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="B442" s="57"/>
-      <c r="C442" s="57"/>
+      <c r="B442" s="55"/>
+      <c r="C442" s="55"/>
     </row>
     <row r="443" spans="1:22" ht="19.5" customHeight="1">
       <c r="A443" s="3">
@@ -24321,7 +24361,7 @@
         <v>72</v>
       </c>
       <c r="U443" s="4">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="V443" s="38" t="s">
         <v>73</v>
@@ -24365,7 +24405,7 @@
         <v>1.95</v>
       </c>
       <c r="N444" s="50">
-        <v>2.79</v>
+        <v>2.7</v>
       </c>
       <c r="O444" s="43" t="s">
         <v>61</v>
@@ -24454,7 +24494,7 @@
         <v>28</v>
       </c>
       <c r="V445" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="446" spans="1:22" ht="19.5" customHeight="1">
@@ -24931,10 +24971,10 @@
       <c r="L455" s="21"/>
       <c r="M455" s="17"/>
       <c r="N455" s="48"/>
-      <c r="O455" s="55" t="s">
+      <c r="O455" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P455" s="55"/>
+      <c r="P455" s="56"/>
       <c r="Q455" s="5"/>
       <c r="T455" s="3"/>
       <c r="V455" s="17"/>
@@ -24949,11 +24989,11 @@
         <v>16</v>
       </c>
       <c r="J456" s="24"/>
-      <c r="K456" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L456" s="56"/>
-      <c r="M456" s="56"/>
+      <c r="K456" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L456" s="57"/>
+      <c r="M456" s="57"/>
       <c r="N456" s="52" t="s">
         <v>23</v>
       </c>
@@ -25107,11 +25147,11 @@
       </c>
     </row>
     <row r="459" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A459" s="57" t="s">
+      <c r="A459" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="B459" s="57"/>
-      <c r="C459" s="57"/>
+      <c r="B459" s="55"/>
+      <c r="C459" s="55"/>
       <c r="D459" s="40"/>
       <c r="E459" s="40"/>
       <c r="F459" s="40"/>
@@ -25222,7 +25262,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="K461" s="4">
-        <v>15.5</v>
+        <v>25.5</v>
       </c>
       <c r="L461" s="4">
         <v>17.559999999999999</v>
@@ -25580,7 +25620,7 @@
         <v>72</v>
       </c>
       <c r="U466" s="4">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="V466" s="38" t="s">
         <v>73</v>
@@ -25645,7 +25685,7 @@
         <v>81</v>
       </c>
       <c r="U467" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="V467" s="38" t="s">
         <v>73</v>
@@ -25782,11 +25822,11 @@
       </c>
     </row>
     <row r="471" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A471" s="57" t="s">
+      <c r="A471" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="B471" s="57"/>
-      <c r="C471" s="57"/>
+      <c r="B471" s="55"/>
+      <c r="C471" s="55"/>
     </row>
     <row r="472" spans="1:22" ht="19.5" customHeight="1">
       <c r="A472" s="3">
@@ -26083,7 +26123,7 @@
         <v>23.8</v>
       </c>
       <c r="L476" s="4">
-        <v>18.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="M476" s="4">
         <v>2.82</v>
@@ -26281,7 +26321,7 @@
         <v>23.1</v>
       </c>
       <c r="L479" s="4">
-        <v>2.04</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="M479" s="4">
         <v>3.34</v>
@@ -26463,10 +26503,10 @@
       <c r="L484" s="21"/>
       <c r="M484" s="17"/>
       <c r="N484" s="48"/>
-      <c r="O484" s="55" t="s">
+      <c r="O484" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P484" s="55"/>
+      <c r="P484" s="56"/>
       <c r="Q484" s="5"/>
       <c r="T484" s="3"/>
       <c r="V484" s="17"/>
@@ -26481,11 +26521,11 @@
         <v>16</v>
       </c>
       <c r="J485" s="24"/>
-      <c r="K485" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L485" s="56"/>
-      <c r="M485" s="56"/>
+      <c r="K485" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L485" s="57"/>
+      <c r="M485" s="57"/>
       <c r="N485" s="52" t="s">
         <v>23</v>
       </c>
@@ -26639,11 +26679,11 @@
       </c>
     </row>
     <row r="488" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A488" s="57" t="s">
+      <c r="A488" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="B488" s="57"/>
-      <c r="C488" s="57"/>
+      <c r="B488" s="55"/>
+      <c r="C488" s="55"/>
       <c r="D488" s="40"/>
       <c r="E488" s="40"/>
       <c r="F488" s="40"/>
@@ -26711,7 +26751,7 @@
         <v>71</v>
       </c>
       <c r="R489" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S489" s="3">
         <v>2</v>
@@ -26776,10 +26816,10 @@
         <v>14</v>
       </c>
       <c r="Q490" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R490" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S490" s="3">
         <v>1</v>
@@ -26847,7 +26887,7 @@
         <v>71</v>
       </c>
       <c r="R491" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S491" s="3">
         <v>2</v>
@@ -26912,7 +26952,7 @@
         <v>71</v>
       </c>
       <c r="R492" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S492" s="3">
         <v>2</v>
@@ -26974,10 +27014,10 @@
         <v>14</v>
       </c>
       <c r="Q493" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R493" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S493" s="3">
         <v>2</v>
@@ -27042,7 +27082,7 @@
         <v>71</v>
       </c>
       <c r="R494" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S494" s="3">
         <v>1</v>
@@ -27107,7 +27147,7 @@
         <v>71</v>
       </c>
       <c r="R495" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S495" s="3">
         <v>2</v>
@@ -27172,7 +27212,7 @@
         <v>71</v>
       </c>
       <c r="R496" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S496" s="3">
         <v>2</v>
@@ -27237,7 +27277,7 @@
         <v>71</v>
       </c>
       <c r="R497" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S497" s="3">
         <v>1</v>
@@ -27302,7 +27342,7 @@
         <v>71</v>
       </c>
       <c r="R498" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S498" s="3">
         <v>1</v>
@@ -27311,18 +27351,18 @@
         <v>78</v>
       </c>
       <c r="U498" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V498" s="26" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="500" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A500" s="57" t="s">
+      <c r="A500" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="B500" s="57"/>
-      <c r="C500" s="57"/>
+      <c r="B500" s="55"/>
+      <c r="C500" s="55"/>
     </row>
     <row r="501" spans="1:23" ht="19.5" customHeight="1">
       <c r="A501" s="3">
@@ -27539,10 +27579,10 @@
         <v>1</v>
       </c>
       <c r="G504" s="3">
-        <v>4.79</v>
+        <v>4.57</v>
       </c>
       <c r="H504" s="3">
-        <v>0.7</v>
+        <v>2.7</v>
       </c>
       <c r="J504" s="4">
         <v>8.9999999999999993E-3</v>
@@ -27554,13 +27594,13 @@
         <v>16.579999999999998</v>
       </c>
       <c r="M504" s="4">
-        <v>2.0699999999999998</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="N504" s="50">
-        <v>2.69</v>
+        <v>2.88</v>
       </c>
       <c r="O504" s="43" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="P504" s="43" t="s">
         <v>14</v>
@@ -27711,7 +27751,7 @@
         <v>77</v>
       </c>
       <c r="W506" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="507" spans="1:23" ht="19.5" customHeight="1">
@@ -27959,7 +27999,7 @@
         <v>14</v>
       </c>
       <c r="Q510" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R510" s="38" t="s">
         <v>71</v>
@@ -27993,10 +28033,10 @@
       <c r="L513" s="21"/>
       <c r="M513" s="17"/>
       <c r="N513" s="48"/>
-      <c r="O513" s="55" t="s">
+      <c r="O513" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P513" s="55"/>
+      <c r="P513" s="56"/>
       <c r="Q513" s="5"/>
       <c r="T513" s="3"/>
       <c r="V513" s="17"/>
@@ -28011,11 +28051,11 @@
         <v>16</v>
       </c>
       <c r="J514" s="24"/>
-      <c r="K514" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L514" s="56"/>
-      <c r="M514" s="56"/>
+      <c r="K514" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L514" s="57"/>
+      <c r="M514" s="57"/>
       <c r="N514" s="52" t="s">
         <v>23</v>
       </c>
@@ -28169,11 +28209,11 @@
       </c>
     </row>
     <row r="517" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A517" s="57" t="s">
+      <c r="A517" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="B517" s="57"/>
-      <c r="C517" s="57"/>
+      <c r="B517" s="55"/>
+      <c r="C517" s="55"/>
       <c r="D517" s="40"/>
       <c r="E517" s="40"/>
       <c r="F517" s="40"/>
@@ -28850,11 +28890,11 @@
       </c>
     </row>
     <row r="529" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A529" s="57" t="s">
+      <c r="A529" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="B529" s="57"/>
-      <c r="C529" s="57"/>
+      <c r="B529" s="55"/>
+      <c r="C529" s="55"/>
     </row>
     <row r="530" spans="1:22" ht="19.5" customHeight="1">
       <c r="A530" s="3">
@@ -29042,7 +29082,7 @@
         <v>2</v>
       </c>
       <c r="T532" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U532" s="4">
         <v>37</v>
@@ -29534,10 +29574,10 @@
       <c r="L542" s="21"/>
       <c r="M542" s="17"/>
       <c r="N542" s="48"/>
-      <c r="O542" s="55" t="s">
+      <c r="O542" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P542" s="55"/>
+      <c r="P542" s="56"/>
       <c r="Q542" s="5"/>
       <c r="T542" s="3"/>
       <c r="V542" s="17"/>
@@ -29552,11 +29592,11 @@
         <v>16</v>
       </c>
       <c r="J543" s="24"/>
-      <c r="K543" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L543" s="56"/>
-      <c r="M543" s="56"/>
+      <c r="K543" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L543" s="57"/>
+      <c r="M543" s="57"/>
       <c r="N543" s="52" t="s">
         <v>23</v>
       </c>
@@ -29710,11 +29750,11 @@
       </c>
     </row>
     <row r="546" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A546" s="57" t="s">
+      <c r="A546" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="B546" s="57"/>
-      <c r="C546" s="57"/>
+      <c r="B546" s="55"/>
+      <c r="C546" s="55"/>
       <c r="D546" s="40"/>
       <c r="E546" s="40"/>
       <c r="F546" s="40"/>
@@ -30189,7 +30229,7 @@
         <v>77</v>
       </c>
       <c r="W553" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="554" spans="1:23" ht="19.5" customHeight="1">
@@ -30394,11 +30434,11 @@
       </c>
     </row>
     <row r="558" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A558" s="57" t="s">
+      <c r="A558" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="B558" s="57"/>
-      <c r="C558" s="57"/>
+      <c r="B558" s="55"/>
+      <c r="C558" s="55"/>
     </row>
     <row r="559" spans="1:23" ht="19.5" customHeight="1">
       <c r="A559" s="3">
@@ -31072,10 +31112,10 @@
       <c r="L571" s="21"/>
       <c r="M571" s="17"/>
       <c r="N571" s="48"/>
-      <c r="O571" s="55" t="s">
+      <c r="O571" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P571" s="55"/>
+      <c r="P571" s="56"/>
       <c r="Q571" s="5"/>
       <c r="T571" s="3"/>
       <c r="V571" s="17"/>
@@ -31090,11 +31130,11 @@
         <v>16</v>
       </c>
       <c r="J572" s="24"/>
-      <c r="K572" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L572" s="56"/>
-      <c r="M572" s="56"/>
+      <c r="K572" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L572" s="57"/>
+      <c r="M572" s="57"/>
       <c r="N572" s="52" t="s">
         <v>23</v>
       </c>
@@ -31248,11 +31288,11 @@
       </c>
     </row>
     <row r="575" spans="1:22" ht="19.5" customHeight="1">
-      <c r="A575" s="57" t="s">
+      <c r="A575" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="B575" s="57"/>
-      <c r="C575" s="57"/>
+      <c r="B575" s="55"/>
+      <c r="C575" s="55"/>
       <c r="D575" s="40"/>
       <c r="E575" s="40"/>
       <c r="F575" s="40"/>
@@ -31629,7 +31669,7 @@
         <v>29.21</v>
       </c>
       <c r="L581" s="4">
-        <v>19.52</v>
+        <v>19.649999999999999</v>
       </c>
       <c r="M581" s="4">
         <v>3.61</v>
@@ -31697,22 +31737,22 @@
         <v>2.9</v>
       </c>
       <c r="N582" s="50">
-        <v>2.86</v>
+        <v>2.64</v>
       </c>
       <c r="O582" s="43" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="P582" s="43" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="Q582" s="38" t="s">
         <v>71</v>
       </c>
       <c r="R582" s="38" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="S582" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T582" s="44" t="s">
         <v>72</v>
@@ -31762,7 +31802,7 @@
         <v>3.37</v>
       </c>
       <c r="N583" s="50">
-        <v>2.89</v>
+        <v>2.86</v>
       </c>
       <c r="O583" s="43" t="s">
         <v>6</v>
@@ -31985,11 +32025,11 @@
       </c>
     </row>
     <row r="588" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A588" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="B588" s="57"/>
-      <c r="C588" s="57"/>
+      <c r="A588" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B588" s="55"/>
+      <c r="C588" s="55"/>
     </row>
     <row r="589" spans="1:23" ht="19.5" customHeight="1">
       <c r="A589" s="3">
@@ -32115,7 +32155,7 @@
         <v>73</v>
       </c>
       <c r="W590" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="591" spans="1:23" ht="19.5" customHeight="1">
@@ -32549,7 +32589,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="N597" s="50">
-        <v>3.31</v>
+        <v>3.02</v>
       </c>
       <c r="O597" s="43" t="s">
         <v>61</v>
@@ -32643,6 +32683,82 @@
     </row>
   </sheetData>
   <mergeCells count="86">
+    <mergeCell ref="O571:P571"/>
+    <mergeCell ref="K572:M572"/>
+    <mergeCell ref="A575:C575"/>
+    <mergeCell ref="A588:C588"/>
+    <mergeCell ref="A517:C517"/>
+    <mergeCell ref="A529:C529"/>
+    <mergeCell ref="O542:P542"/>
+    <mergeCell ref="K543:M543"/>
+    <mergeCell ref="A546:C546"/>
+    <mergeCell ref="A558:C558"/>
+    <mergeCell ref="O484:P484"/>
+    <mergeCell ref="K485:M485"/>
+    <mergeCell ref="A488:C488"/>
+    <mergeCell ref="A500:C500"/>
+    <mergeCell ref="O513:P513"/>
+    <mergeCell ref="K514:M514"/>
+    <mergeCell ref="A430:C430"/>
+    <mergeCell ref="A442:C442"/>
+    <mergeCell ref="O455:P455"/>
+    <mergeCell ref="K456:M456"/>
+    <mergeCell ref="A459:C459"/>
+    <mergeCell ref="A471:C471"/>
+    <mergeCell ref="O397:P397"/>
+    <mergeCell ref="K398:M398"/>
+    <mergeCell ref="A401:C401"/>
+    <mergeCell ref="A413:C413"/>
+    <mergeCell ref="O426:P426"/>
+    <mergeCell ref="K427:M427"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="A22:T22"/>
+    <mergeCell ref="A4:T4"/>
+    <mergeCell ref="A3:T3"/>
+    <mergeCell ref="A20:T20"/>
+    <mergeCell ref="A21:T21"/>
+    <mergeCell ref="A10:T10"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="O60:P60"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="O88:P88"/>
+    <mergeCell ref="K89:M89"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="A232:C232"/>
+    <mergeCell ref="A244:C244"/>
+    <mergeCell ref="O116:P116"/>
+    <mergeCell ref="K117:M117"/>
+    <mergeCell ref="A120:C120"/>
+    <mergeCell ref="A132:C132"/>
+    <mergeCell ref="O144:P144"/>
+    <mergeCell ref="K145:M145"/>
+    <mergeCell ref="A148:C148"/>
+    <mergeCell ref="A160:C160"/>
+    <mergeCell ref="O172:P172"/>
+    <mergeCell ref="K173:M173"/>
+    <mergeCell ref="A176:C176"/>
+    <mergeCell ref="A188:C188"/>
+    <mergeCell ref="O200:P200"/>
+    <mergeCell ref="K201:M201"/>
+    <mergeCell ref="A204:C204"/>
+    <mergeCell ref="A216:C216"/>
+    <mergeCell ref="O228:P228"/>
+    <mergeCell ref="K229:M229"/>
+    <mergeCell ref="O256:P256"/>
+    <mergeCell ref="K257:M257"/>
+    <mergeCell ref="A260:C260"/>
+    <mergeCell ref="A272:C272"/>
+    <mergeCell ref="O284:P284"/>
+    <mergeCell ref="K285:M285"/>
+    <mergeCell ref="A288:C288"/>
+    <mergeCell ref="A300:C300"/>
+    <mergeCell ref="O312:P312"/>
+    <mergeCell ref="K313:M313"/>
     <mergeCell ref="A316:C316"/>
     <mergeCell ref="A328:C328"/>
     <mergeCell ref="A372:C372"/>
@@ -32653,82 +32769,6 @@
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="O368:P368"/>
     <mergeCell ref="K369:M369"/>
-    <mergeCell ref="O284:P284"/>
-    <mergeCell ref="K285:M285"/>
-    <mergeCell ref="A288:C288"/>
-    <mergeCell ref="A300:C300"/>
-    <mergeCell ref="O312:P312"/>
-    <mergeCell ref="K313:M313"/>
-    <mergeCell ref="O228:P228"/>
-    <mergeCell ref="K229:M229"/>
-    <mergeCell ref="O256:P256"/>
-    <mergeCell ref="K257:M257"/>
-    <mergeCell ref="A260:C260"/>
-    <mergeCell ref="A272:C272"/>
-    <mergeCell ref="A176:C176"/>
-    <mergeCell ref="A188:C188"/>
-    <mergeCell ref="O200:P200"/>
-    <mergeCell ref="K201:M201"/>
-    <mergeCell ref="A204:C204"/>
-    <mergeCell ref="A216:C216"/>
-    <mergeCell ref="O144:P144"/>
-    <mergeCell ref="K145:M145"/>
-    <mergeCell ref="A148:C148"/>
-    <mergeCell ref="A160:C160"/>
-    <mergeCell ref="O172:P172"/>
-    <mergeCell ref="K173:M173"/>
-    <mergeCell ref="O88:P88"/>
-    <mergeCell ref="K89:M89"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="A232:C232"/>
-    <mergeCell ref="A244:C244"/>
-    <mergeCell ref="O116:P116"/>
-    <mergeCell ref="K117:M117"/>
-    <mergeCell ref="A120:C120"/>
-    <mergeCell ref="A132:C132"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="O60:P60"/>
-    <mergeCell ref="K61:M61"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="A22:T22"/>
-    <mergeCell ref="A4:T4"/>
-    <mergeCell ref="A3:T3"/>
-    <mergeCell ref="A20:T20"/>
-    <mergeCell ref="A21:T21"/>
-    <mergeCell ref="A10:T10"/>
-    <mergeCell ref="O397:P397"/>
-    <mergeCell ref="K398:M398"/>
-    <mergeCell ref="A401:C401"/>
-    <mergeCell ref="A413:C413"/>
-    <mergeCell ref="O426:P426"/>
-    <mergeCell ref="K427:M427"/>
-    <mergeCell ref="A430:C430"/>
-    <mergeCell ref="A442:C442"/>
-    <mergeCell ref="O455:P455"/>
-    <mergeCell ref="K456:M456"/>
-    <mergeCell ref="A459:C459"/>
-    <mergeCell ref="A471:C471"/>
-    <mergeCell ref="O484:P484"/>
-    <mergeCell ref="K485:M485"/>
-    <mergeCell ref="A488:C488"/>
-    <mergeCell ref="A500:C500"/>
-    <mergeCell ref="O513:P513"/>
-    <mergeCell ref="K514:M514"/>
-    <mergeCell ref="O571:P571"/>
-    <mergeCell ref="K572:M572"/>
-    <mergeCell ref="A575:C575"/>
-    <mergeCell ref="A588:C588"/>
-    <mergeCell ref="A517:C517"/>
-    <mergeCell ref="A529:C529"/>
-    <mergeCell ref="O542:P542"/>
-    <mergeCell ref="K543:M543"/>
-    <mergeCell ref="A546:C546"/>
-    <mergeCell ref="A558:C558"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions gridLines="1"/>

</xml_diff>